<commit_message>
quang update lan 2
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>IdHD</t>
   </si>
   <si>
-    <t>Loại</t>
-  </si>
-  <si>
     <t>Tên dịch vụ</t>
   </si>
   <si>
@@ -56,19 +53,58 @@
     <t>P015693</t>
   </si>
   <si>
-    <t>2023-12-06 15:44:00</t>
+    <t>2023-12-07 08:16:00</t>
+  </si>
+  <si>
+    <t>2023-12-23 14:16:00</t>
+  </si>
+  <si>
+    <t>Đã thanh toán</t>
+  </si>
+  <si>
+    <t>2023-12-12 22:01:06</t>
+  </si>
+  <si>
+    <t>2023-12-13 22:00:00</t>
   </si>
   <si>
     <t>Chưa thanh toán</t>
   </si>
   <si>
-    <t>2023-12-07 08:16:40</t>
-  </si>
-  <si>
-    <t>2023-12-08 14:16:40</t>
-  </si>
-  <si>
-    <t>Đã thanh toán</t>
+    <t>2023-12-12 22:01:47</t>
+  </si>
+  <si>
+    <t>2023-12-21 22:01:00</t>
+  </si>
+  <si>
+    <t>P096400</t>
+  </si>
+  <si>
+    <t>2023-12-12 16:06:54</t>
+  </si>
+  <si>
+    <t>2023-12-12 16:09:33</t>
+  </si>
+  <si>
+    <t>2023-12-13 22:09:34</t>
+  </si>
+  <si>
+    <t>2023-12-16 16:00:38</t>
+  </si>
+  <si>
+    <t>2023-12-09 15:59:00</t>
+  </si>
+  <si>
+    <t>2023-12-16 16:19:22</t>
+  </si>
+  <si>
+    <t>2023-12-16 17:05:46</t>
+  </si>
+  <si>
+    <t>2023-12-16 17:41:18</t>
+  </si>
+  <si>
+    <t>2023-12-22 17:41:00</t>
   </si>
 </sst>
 </file>
@@ -419,7 +455,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,67 +464,64 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="true" style="0"/>
+    <col min="3" max="3" width="50" customWidth="true" style="0"/>
     <col min="2" max="2" width="50" customWidth="true" style="0"/>
-    <col min="3" max="3" width="50" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="0">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0"/>
       <c r="I2" s="0">
-        <v>123213123</v>
+        <v>10000</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>14</v>
@@ -496,33 +529,219 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="0">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0">
-        <v>23</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0">
+        <v>1111</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="0">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0">
+        <v>123</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="0">
         <v>15</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0">
+        <v>312</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0">
+        <v>111111</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="0">
         <v>16</v>
       </c>
-      <c r="I3" s="0">
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0">
+        <v>312</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="0">
+        <v>123123</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="0">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0">
+        <v>312</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0">
         <v>10000</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J7" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="0">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0">
+        <v>312</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0">
+        <v>10000</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="0">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0">
+        <v>312</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0">
+        <v>10005</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="0">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0">
+        <v>312</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0">
+        <v>123123</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>